<commit_message>
opencv 및 matplotlib 교육
</commit_message>
<xml_diff>
--- a/0509/static/result.xlsx
+++ b/0509/static/result.xlsx
@@ -424,7 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>봄 소풍의 설렘을 다시 한번!</t>
+          <t>아프리카 최빈국 말라위 청년에게 자립 기회를!</t>
         </is>
       </c>
     </row>
@@ -438,56 +438,56 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>8살 니샤의 학교는 '일하지 않아도 되는 곳'</t>
+          <t>“집에 있으면 뭐하나... 여기 와야 재밌지.”</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1,004개 목도리를 만들어 온기를 전달할게요!</t>
+          <t>우리는 함께 먹을수록 단단해진다</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>물속에 있으면 엄마 품처럼 따뜻해요~</t>
+          <t>철수의 꿈을 함께 찾아주세요.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>자동심장충격기로 골든타임을 지켜주세요</t>
+          <t>우리 집을 만들어주세요!</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>할미공주 어르신들의 성장을 응원해 주세요!</t>
+          <t>6.25참전 유공자분들께 지팡이를 전달해 주세요</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>석현이의 꿈은 가족을 지켜주는 태권도 선수!</t>
+          <t>따뜻한 한 끼 밥상, 나눔으로 배부른 보통 일상</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>한부모가정에 건강하고 안전한 여름 선물하기⛱️</t>
+          <t>“우리는 경로당 아니면 갈 데가 없어.”</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>뇌성마비 장애인의 안전 지킴이가 되어주세요!</t>
+          <t>올바른 장애 첫인상을 함께 만들어요</t>
         </is>
       </c>
     </row>

</xml_diff>